<commit_message>
New commit at 2023-02-08 13:53:19.086152
</commit_message>
<xml_diff>
--- a/db/procedures/procedures.xlsx
+++ b/db/procedures/procedures.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="20880" windowHeight="8595" activeTab="2"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="20880" windowHeight="8595" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="account procedure" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>NAME</t>
   </si>
@@ -122,9 +122,6 @@
     <t xml:space="preserve">
 1. table_name VARCHAR(255)
 2. table_alias VARCHAR(255)</t>
-  </si>
-  <si>
-    <t>Thêm một bảng mới vào cơ sở dữ liệu và trigger tạo một bảng mới ( Trigger sẽ được viết sau ). Lưu ý, đối số table_alias không thể tự tạo bằng thuật toán MySQL nên hãy tạo bằng code Nodejs rồi truyền vào proc như một đối số bình thường.</t>
   </si>
   <si>
     <t>table_modify</t>
@@ -169,6 +166,21 @@
   </si>
   <si>
     <t>modify_field</t>
+  </si>
+  <si>
+    <t>Cập nhật trạng thái của trường với ID = field_id</t>
+  </si>
+  <si>
+    <t>drop_field</t>
+  </si>
+  <si>
+    <t>1. field_id INT(255)</t>
+  </si>
+  <si>
+    <t>Xóa trường nhe quí dị</t>
+  </si>
+  <si>
+    <t>Thêm một bảng mới vào cơ sở dữ liệu và trigger tạo một bảng mới (Với một trường ID khóa chính nội tại). Lưu ý, đối số table_alias không thể tự tạo bằng thuật toán MySQL nên hãy tạo bằng code Nodejs rồi truyền vào proc như một đối số bình thường.</t>
   </si>
 </sst>
 </file>
@@ -818,8 +830,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A3:F45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -866,22 +878,22 @@
         <v>19</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="69" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="4"/>
     </row>
@@ -1092,11 +1104,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="28.42578125" style="2" customWidth="1"/>
@@ -1108,7 +1120,7 @@
   <sheetData>
     <row r="3" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1131,226 +1143,234 @@
     <row r="5" spans="1:6" ht="155.25" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="138" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="69" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D45" s="3"/>
     </row>
   </sheetData>

</xml_diff>